<commit_message>
Project with AI  LLM + RAG(Pinecone) + FastAPI + Postgres Cache
</commit_message>
<xml_diff>
--- a/base_veiculos.xlsx
+++ b/base_veiculos.xlsx
@@ -488,108 +488,108 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Creta</t>
+          <t>Cruze</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2016</v>
+        <v>2021</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>71886</v>
+        <v>84035</v>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>78210</v>
+        <v>49622</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EcoSport</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>69879</v>
+        <v>20693</v>
       </c>
       <c r="H3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>38801</v>
+        <v>113077</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Yaris</t>
+          <t>T-Cross</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -599,58 +599,58 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>81129</v>
+        <v>10263</v>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>111805</v>
+        <v>102636</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>18657</v>
+        <v>69484</v>
       </c>
       <c r="H5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -658,75 +658,75 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>117098</v>
+        <v>114347</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Gol</t>
+          <t>Tracker</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>45222</v>
+        <v>60338</v>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>112151</v>
+        <v>62937</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cruze</t>
+          <t>Gol</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -735,33 +735,33 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>36876</v>
+        <v>78584</v>
       </c>
       <c r="H7" t="n">
         <v>2</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>80004</v>
+        <v>96489</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Creta</t>
+          <t>Yaris</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -779,18 +779,18 @@
         </is>
       </c>
       <c r="G8" t="n">
-        <v>12777</v>
+        <v>40615</v>
       </c>
       <c r="H8" t="n">
         <v>4</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>108020</v>
+        <v>78265</v>
       </c>
     </row>
     <row r="9">
@@ -805,11 +805,11 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -823,10 +823,10 @@
         </is>
       </c>
       <c r="G9" t="n">
-        <v>36813</v>
+        <v>25829</v>
       </c>
       <c r="H9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -834,31 +834,31 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>50125</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>HR-V</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -867,18 +867,18 @@
         </is>
       </c>
       <c r="G10" t="n">
-        <v>21415</v>
+        <v>46907</v>
       </c>
       <c r="H10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>67417</v>
+        <v>76396</v>
       </c>
     </row>
     <row r="11">
@@ -889,20 +889,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Creta</t>
+          <t>Tucson</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -911,62 +911,62 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>67024</v>
+        <v>75621</v>
       </c>
       <c r="H11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>36026</v>
+        <v>53265</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cruze</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>73682</v>
+        <v>52450</v>
       </c>
       <c r="H12" t="n">
         <v>4</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>57259</v>
+        <v>88885</v>
       </c>
     </row>
     <row r="13">
@@ -977,51 +977,51 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>EcoSport</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>39721</v>
+        <v>41079</v>
       </c>
       <c r="H13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>112575</v>
+        <v>39509</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>HB20</t>
+          <t>Cruze</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1029,7 +1029,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1039,41 +1039,41 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>32529</v>
+        <v>39022</v>
       </c>
       <c r="H14" t="n">
         <v>4</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J14" t="n">
-        <v>92347</v>
+        <v>87104</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Fiesta</t>
+          <t>Hilux</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1083,46 +1083,46 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>15748</v>
+        <v>52561</v>
       </c>
       <c r="H15" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>51776</v>
+        <v>77326</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cruze</t>
+          <t>EcoSport</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1131,33 +1131,33 @@
         </is>
       </c>
       <c r="G16" t="n">
-        <v>17523</v>
+        <v>77973</v>
       </c>
       <c r="H16" t="n">
         <v>4</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>117736</v>
+        <v>87877</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Yaris</t>
+          <t>Polo</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2015</v>
+        <v>2023</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1175,29 +1175,29 @@
         </is>
       </c>
       <c r="G17" t="n">
-        <v>53703</v>
+        <v>36010</v>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J17" t="n">
-        <v>105133</v>
+        <v>111592</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>T-Cross</t>
+          <t>Hilux</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1210,19 +1210,19 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>21596</v>
+        <v>73535</v>
       </c>
       <c r="H18" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1230,26 +1230,26 @@
         </is>
       </c>
       <c r="J18" t="n">
-        <v>47539</v>
+        <v>35424</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Tracker</t>
+          <t>Hilux</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1259,22 +1259,22 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>61930</v>
+        <v>54196</v>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J19" t="n">
-        <v>86985</v>
+        <v>86085</v>
       </c>
     </row>
     <row r="20">
@@ -1285,51 +1285,51 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Fiesta</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>2015</v>
+        <v>2022</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>50551</v>
+        <v>37323</v>
       </c>
       <c r="H20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J20" t="n">
-        <v>76536</v>
+        <v>118098</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>T-Cross</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1337,7 +1337,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1347,37 +1347,37 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>61068</v>
+        <v>22369</v>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J21" t="n">
-        <v>67912</v>
+        <v>72284</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>EcoSport</t>
+          <t>Onix</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1395,33 +1395,33 @@
         </is>
       </c>
       <c r="G22" t="n">
-        <v>51275</v>
+        <v>31734</v>
       </c>
       <c r="H22" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J22" t="n">
-        <v>50386</v>
+        <v>112677</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>EcoSport</t>
+          <t>HR-V</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1430,19 +1430,19 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>41105</v>
+        <v>51398</v>
       </c>
       <c r="H23" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1450,22 +1450,22 @@
         </is>
       </c>
       <c r="J23" t="n">
-        <v>58331</v>
+        <v>99070</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2016</v>
+        <v>2023</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1479,41 +1479,41 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>57592</v>
+        <v>22141</v>
       </c>
       <c r="H24" t="n">
         <v>2</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J24" t="n">
-        <v>43077</v>
+        <v>91641</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fit</t>
+          <t>Polo</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1527,33 +1527,33 @@
         </is>
       </c>
       <c r="G25" t="n">
-        <v>52995</v>
+        <v>42698</v>
       </c>
       <c r="H25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J25" t="n">
-        <v>38271</v>
+        <v>38792</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Fit</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1562,7 +1562,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1571,51 +1571,51 @@
         </is>
       </c>
       <c r="G26" t="n">
-        <v>61094</v>
+        <v>87446</v>
       </c>
       <c r="H26" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J26" t="n">
-        <v>59378</v>
+        <v>117887</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>HR-V</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>41055</v>
+        <v>82038</v>
       </c>
       <c r="H27" t="n">
         <v>2</v>
@@ -1626,22 +1626,22 @@
         </is>
       </c>
       <c r="J27" t="n">
-        <v>119470</v>
+        <v>74532</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>T-Cross</t>
+          <t>HB20</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2017</v>
+        <v>2019</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1650,51 +1650,51 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>84064</v>
+        <v>41570</v>
       </c>
       <c r="H28" t="n">
         <v>2</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J28" t="n">
-        <v>82271</v>
+        <v>42420</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>HB20</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1703,81 +1703,81 @@
         </is>
       </c>
       <c r="G29" t="n">
-        <v>25489</v>
+        <v>44998</v>
       </c>
       <c r="H29" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J29" t="n">
-        <v>35631</v>
+        <v>67230</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Gol</t>
+          <t>HR-V</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>39023</v>
+        <v>85222</v>
       </c>
       <c r="H30" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J30" t="n">
-        <v>81371</v>
+        <v>88665</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Cruze</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1787,46 +1787,46 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>16136</v>
+        <v>34163</v>
       </c>
       <c r="H31" t="n">
         <v>2</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J31" t="n">
-        <v>93016</v>
+        <v>96211</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>T-Cross</t>
+          <t>HB20</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1835,10 +1835,10 @@
         </is>
       </c>
       <c r="G32" t="n">
-        <v>52047</v>
+        <v>11100</v>
       </c>
       <c r="H32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -1846,26 +1846,26 @@
         </is>
       </c>
       <c r="J32" t="n">
-        <v>113081</v>
+        <v>78135</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>EcoSport</t>
+          <t>Polo</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1879,10 +1879,10 @@
         </is>
       </c>
       <c r="G33" t="n">
-        <v>55840</v>
+        <v>71353</v>
       </c>
       <c r="H33" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="J33" t="n">
-        <v>56805</v>
+        <v>77889</v>
       </c>
     </row>
     <row r="34">
@@ -1905,16 +1905,16 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1923,10 +1923,10 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>14264</v>
+        <v>82235</v>
       </c>
       <c r="H34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -1934,26 +1934,26 @@
         </is>
       </c>
       <c r="J34" t="n">
-        <v>53233</v>
+        <v>77993</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Gol</t>
+          <t>Tracker</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1963,169 +1963,169 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>57465</v>
+        <v>56448</v>
       </c>
       <c r="H35" t="n">
         <v>4</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J35" t="n">
-        <v>79475</v>
+        <v>108731</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Gol</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>61553</v>
+        <v>41363</v>
       </c>
       <c r="H36" t="n">
         <v>2</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J36" t="n">
-        <v>94099</v>
+        <v>107986</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Creta</t>
+          <t>Tracker</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>40067</v>
+        <v>83671</v>
       </c>
       <c r="H37" t="n">
         <v>4</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J37" t="n">
-        <v>60951</v>
+        <v>85995</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Tucson</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>14768</v>
+        <v>77229</v>
       </c>
       <c r="H38" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J38" t="n">
-        <v>110363</v>
+        <v>91279</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Cruze</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2143,37 +2143,37 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>63373</v>
+        <v>33285</v>
       </c>
       <c r="H39" t="n">
         <v>2</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J39" t="n">
-        <v>78732</v>
+        <v>67349</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Fiesta</t>
+          <t>Creta</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2183,129 +2183,129 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>67367</v>
+        <v>82751</v>
       </c>
       <c r="H40" t="n">
         <v>2</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J40" t="n">
-        <v>75178</v>
+        <v>64911</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>HR-V</t>
+          <t>Tucson</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>60566</v>
+        <v>82048</v>
       </c>
       <c r="H41" t="n">
         <v>4</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J41" t="n">
-        <v>70257</v>
+        <v>63855</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Hilux</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2023</v>
+        <v>2016</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>20299</v>
+        <v>82074</v>
       </c>
       <c r="H42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J42" t="n">
-        <v>88893</v>
+        <v>46940</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2315,33 +2315,33 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>40388</v>
+        <v>76380</v>
       </c>
       <c r="H43" t="n">
         <v>2</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J43" t="n">
-        <v>52209</v>
+        <v>58549</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Corolla</t>
+          <t>HB20</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2359,41 +2359,41 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>32470</v>
+        <v>81471</v>
       </c>
       <c r="H44" t="n">
         <v>2</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J44" t="n">
-        <v>39427</v>
+        <v>60913</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Fiesta</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2407,42 +2407,42 @@
         </is>
       </c>
       <c r="G45" t="n">
-        <v>26050</v>
+        <v>15795</v>
       </c>
       <c r="H45" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J45" t="n">
-        <v>97666</v>
+        <v>78197</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Creta</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2451,51 +2451,51 @@
         </is>
       </c>
       <c r="G46" t="n">
-        <v>89215</v>
+        <v>65205</v>
       </c>
       <c r="H46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J46" t="n">
-        <v>41871</v>
+        <v>35784</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>HB20</t>
+          <t>Polo</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>86482</v>
+        <v>88158</v>
       </c>
       <c r="H47" t="n">
         <v>2</v>
@@ -2506,22 +2506,22 @@
         </is>
       </c>
       <c r="J47" t="n">
-        <v>96265</v>
+        <v>93872</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Hilux</t>
+          <t>Creta</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -2530,7 +2530,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2539,7 +2539,7 @@
         </is>
       </c>
       <c r="G48" t="n">
-        <v>77484</v>
+        <v>86294</v>
       </c>
       <c r="H48" t="n">
         <v>2</v>
@@ -2550,7 +2550,7 @@
         </is>
       </c>
       <c r="J48" t="n">
-        <v>65129</v>
+        <v>91406</v>
       </c>
     </row>
     <row r="49">
@@ -2561,40 +2561,40 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Polo</t>
+          <t>Gol</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>2016</v>
+        <v>2023</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>78681</v>
+        <v>18033</v>
       </c>
       <c r="H49" t="n">
         <v>2</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J49" t="n">
-        <v>88056</v>
+        <v>106040</v>
       </c>
     </row>
     <row r="50">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Cruze</t>
+          <t>Onix</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -2613,32 +2613,32 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>79419</v>
+        <v>77179</v>
       </c>
       <c r="H50" t="n">
         <v>2</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J50" t="n">
-        <v>93166</v>
+        <v>77081</v>
       </c>
     </row>
     <row r="51">
@@ -2649,15 +2649,15 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Fiesta</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2671,51 +2671,51 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>68805</v>
+        <v>38551</v>
       </c>
       <c r="H51" t="n">
         <v>2</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J51" t="n">
-        <v>105850</v>
+        <v>56735</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Civic</t>
+          <t>Tracker</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>12168</v>
+        <v>58568</v>
       </c>
       <c r="H52" t="n">
         <v>4</v>
@@ -2726,70 +2726,70 @@
         </is>
       </c>
       <c r="J52" t="n">
-        <v>71969</v>
+        <v>101928</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Creta</t>
+          <t>Cruze</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>28085</v>
+        <v>63516</v>
       </c>
       <c r="H53" t="n">
         <v>2</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J53" t="n">
-        <v>45177</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>HB20</t>
+          <t>Gol</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2799,41 +2799,41 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>27875</v>
+        <v>89866</v>
       </c>
       <c r="H54" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J54" t="n">
-        <v>82388</v>
+        <v>67659</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Fit</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2843,22 +2843,22 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>28441</v>
+        <v>68985</v>
       </c>
       <c r="H55" t="n">
         <v>2</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J55" t="n">
-        <v>119210</v>
+        <v>116180</v>
       </c>
     </row>
     <row r="56">
@@ -2869,11 +2869,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Tracker</t>
+          <t>Onix</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -2882,16 +2882,16 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>74475</v>
+        <v>72925</v>
       </c>
       <c r="H56" t="n">
         <v>4</v>
@@ -2902,18 +2902,18 @@
         </is>
       </c>
       <c r="J56" t="n">
-        <v>55159</v>
+        <v>116491</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Tracker</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -2926,38 +2926,38 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>20356</v>
+        <v>30879</v>
       </c>
       <c r="H57" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J57" t="n">
-        <v>46675</v>
+        <v>95918</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Gol</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -2970,7 +2970,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2979,42 +2979,42 @@
         </is>
       </c>
       <c r="G58" t="n">
-        <v>18964</v>
+        <v>32386</v>
       </c>
       <c r="H58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J58" t="n">
-        <v>58443</v>
+        <v>60687</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Onix</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -3023,54 +3023,54 @@
         </is>
       </c>
       <c r="G59" t="n">
-        <v>16391</v>
+        <v>83231</v>
       </c>
       <c r="H59" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J59" t="n">
-        <v>76758</v>
+        <v>35021</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Fiesta</t>
+          <t>Tracker</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>33924</v>
+        <v>40271</v>
       </c>
       <c r="H60" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
@@ -3078,66 +3078,66 @@
         </is>
       </c>
       <c r="J60" t="n">
-        <v>68205</v>
+        <v>61455</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Polo</t>
+          <t>Fit</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2023</v>
+        <v>2015</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>74726</v>
+        <v>72071</v>
       </c>
       <c r="H61" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J61" t="n">
-        <v>103218</v>
+        <v>64109</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Chevrolet</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Fit</t>
+          <t>Cruze</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -3146,7 +3146,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -3155,29 +3155,29 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>38340</v>
+        <v>30224</v>
       </c>
       <c r="H62" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J62" t="n">
-        <v>106419</v>
+        <v>110399</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Tracker</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -3185,12 +3185,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3199,86 +3199,86 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>68775</v>
+        <v>26574</v>
       </c>
       <c r="H63" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J63" t="n">
-        <v>88953</v>
+        <v>115212</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Onix</t>
+          <t>Fiesta</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>39610</v>
+        <v>29036</v>
       </c>
       <c r="H64" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J64" t="n">
-        <v>57225</v>
+        <v>67632</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>T-Cross</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3287,73 +3287,73 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>66942</v>
+        <v>40128</v>
       </c>
       <c r="H65" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J65" t="n">
-        <v>90085</v>
+        <v>84075</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Gol</t>
+          <t>HR-V</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>22862</v>
+        <v>80383</v>
       </c>
       <c r="H66" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J66" t="n">
-        <v>69916</v>
+        <v>91719</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Onix</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3375,29 +3375,29 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>51608</v>
+        <v>30966</v>
       </c>
       <c r="H67" t="n">
         <v>2</v>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J67" t="n">
-        <v>37703</v>
+        <v>101678</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>T-Cross</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -3419,81 +3419,81 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>62438</v>
+        <v>71636</v>
       </c>
       <c r="H68" t="n">
         <v>2</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J68" t="n">
-        <v>90995</v>
+        <v>43094</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G69" t="n">
-        <v>71608</v>
+        <v>89140</v>
       </c>
       <c r="H69" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J69" t="n">
-        <v>109400</v>
+        <v>117333</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>EcoSport</t>
+          <t>Fit</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3507,18 +3507,18 @@
         </is>
       </c>
       <c r="G70" t="n">
-        <v>49051</v>
+        <v>16009</v>
       </c>
       <c r="H70" t="n">
         <v>2</v>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J70" t="n">
-        <v>106111</v>
+        <v>106197</v>
       </c>
     </row>
     <row r="71">
@@ -3529,40 +3529,40 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Gol</t>
+          <t>Polo</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G71" t="n">
-        <v>82994</v>
+        <v>43188</v>
       </c>
       <c r="H71" t="n">
         <v>4</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J71" t="n">
-        <v>118177</v>
+        <v>56343</v>
       </c>
     </row>
     <row r="72">
@@ -3577,124 +3577,124 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>60490</v>
+        <v>37630</v>
       </c>
       <c r="H72" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J72" t="n">
-        <v>99804</v>
+        <v>92469</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>HB20</t>
+          <t>Fiesta</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>2017</v>
+        <v>2023</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>65190</v>
+        <v>42298</v>
       </c>
       <c r="H73" t="n">
         <v>4</v>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J73" t="n">
-        <v>81157</v>
+        <v>83381</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Tucson</t>
+          <t>Fiesta</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2023</v>
+        <v>2016</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>47551</v>
+        <v>66893</v>
       </c>
       <c r="H74" t="n">
         <v>2</v>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J74" t="n">
-        <v>61084</v>
+        <v>40167</v>
       </c>
     </row>
     <row r="75">
@@ -3705,99 +3705,99 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>HB20</t>
+          <t>Creta</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>68980</v>
+        <v>62799</v>
       </c>
       <c r="H75" t="n">
         <v>2</v>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J75" t="n">
-        <v>39234</v>
+        <v>64525</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Hyundai</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>HB20</t>
+          <t>EcoSport</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>30402</v>
+        <v>38311</v>
       </c>
       <c r="H76" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J76" t="n">
-        <v>65467</v>
+        <v>52312</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>T-Cross</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -3811,154 +3811,154 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G77" t="n">
-        <v>20728</v>
+        <v>14836</v>
       </c>
       <c r="H77" t="n">
         <v>4</v>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J77" t="n">
-        <v>96275</v>
+        <v>116519</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Yaris</t>
+          <t>Polo</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G78" t="n">
-        <v>33410</v>
+        <v>47364</v>
       </c>
       <c r="H78" t="n">
         <v>4</v>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>azul</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J78" t="n">
-        <v>99240</v>
+        <v>61623</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>T-Cross</t>
+          <t>Ka</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>36598</v>
+        <v>39664</v>
       </c>
       <c r="H79" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J79" t="n">
-        <v>55231</v>
+        <v>107484</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Fit</t>
+          <t>Hilux</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>66031</v>
+        <v>35037</v>
       </c>
       <c r="H80" t="n">
         <v>4</v>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J80" t="n">
-        <v>99879</v>
+        <v>62084</v>
       </c>
     </row>
     <row r="81">
@@ -3969,15 +3969,15 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Gol</t>
+          <t>Polo</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -3987,14 +3987,14 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>44630</v>
+        <v>53935</v>
       </c>
       <c r="H81" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I81" t="inlineStr">
         <is>
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="J81" t="n">
-        <v>84552</v>
+        <v>112234</v>
       </c>
     </row>
     <row r="82">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Gol</t>
+          <t>T-Cross</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -4031,14 +4031,14 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>57704</v>
+        <v>21100</v>
       </c>
       <c r="H82" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I82" t="inlineStr">
         <is>
@@ -4046,7 +4046,7 @@
         </is>
       </c>
       <c r="J82" t="n">
-        <v>44123</v>
+        <v>84326</v>
       </c>
     </row>
     <row r="83">
@@ -4057,11 +4057,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>HR-V</t>
+          <t>Fit</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -4070,42 +4070,42 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>63473</v>
+        <v>56925</v>
       </c>
       <c r="H83" t="n">
         <v>2</v>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J83" t="n">
-        <v>90548</v>
+        <v>106300</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Fit</t>
+          <t>EcoSport</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -4119,22 +4119,22 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>18496</v>
+        <v>33034</v>
       </c>
       <c r="H84" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>prata</t>
         </is>
       </c>
       <c r="J84" t="n">
-        <v>88022</v>
+        <v>65065</v>
       </c>
     </row>
     <row r="85">
@@ -4145,15 +4145,15 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Fit</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -4163,213 +4163,213 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>35044</v>
+        <v>54139</v>
       </c>
       <c r="H85" t="n">
         <v>2</v>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J85" t="n">
-        <v>41642</v>
+        <v>63831</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Polo</t>
+          <t>Yaris</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G86" t="n">
-        <v>57884</v>
+        <v>38144</v>
       </c>
       <c r="H86" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J86" t="n">
-        <v>42929</v>
+        <v>66034</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Cruze</t>
+          <t>HR-V</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G87" t="n">
-        <v>30589</v>
+        <v>16891</v>
       </c>
       <c r="H87" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>azul</t>
         </is>
       </c>
       <c r="J87" t="n">
-        <v>53279</v>
+        <v>52007</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>T-Cross</t>
+          <t>HR-V</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>12903</v>
+        <v>84325</v>
       </c>
       <c r="H88" t="n">
         <v>2</v>
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J88" t="n">
-        <v>106693</v>
+        <v>99778</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Honda</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>HR-V</t>
+          <t>Polo</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G89" t="n">
-        <v>60510</v>
+        <v>75181</v>
       </c>
       <c r="H89" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J89" t="n">
-        <v>81039</v>
+        <v>44345</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Polo</t>
+          <t>Corolla</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -4378,7 +4378,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -4387,42 +4387,42 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>15684</v>
+        <v>27961</v>
       </c>
       <c r="H90" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>preto</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J90" t="n">
-        <v>101783</v>
+        <v>93504</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Honda</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Tracker</t>
+          <t>Civic</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.4</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -4431,33 +4431,33 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>68059</v>
+        <v>77622</v>
       </c>
       <c r="H91" t="n">
         <v>4</v>
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>branco</t>
         </is>
       </c>
       <c r="J91" t="n">
-        <v>97071</v>
+        <v>92715</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Fiesta</t>
+          <t>T-Cross</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -4466,19 +4466,19 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G92" t="n">
-        <v>87080</v>
+        <v>53466</v>
       </c>
       <c r="H92" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I92" t="inlineStr">
         <is>
@@ -4486,18 +4486,18 @@
         </is>
       </c>
       <c r="J92" t="n">
-        <v>78800</v>
+        <v>40852</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Ka</t>
+          <t>HB20</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -4505,12 +4505,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -4519,10 +4519,10 @@
         </is>
       </c>
       <c r="G93" t="n">
-        <v>73257</v>
+        <v>88225</v>
       </c>
       <c r="H93" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I93" t="inlineStr">
         <is>
@@ -4530,7 +4530,7 @@
         </is>
       </c>
       <c r="J93" t="n">
-        <v>66902</v>
+        <v>115844</v>
       </c>
     </row>
     <row r="94">
@@ -4541,20 +4541,20 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Fit</t>
+          <t>HR-V</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -4563,10 +4563,10 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>45100</v>
+        <v>75500</v>
       </c>
       <c r="H94" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I94" t="inlineStr">
         <is>
@@ -4574,22 +4574,22 @@
         </is>
       </c>
       <c r="J94" t="n">
-        <v>36801</v>
+        <v>57573</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Ford</t>
+          <t>Volkswagen</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>EcoSport</t>
+          <t>T-Cross</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -4598,7 +4598,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -4607,18 +4607,18 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>62165</v>
+        <v>70639</v>
       </c>
       <c r="H95" t="n">
         <v>4</v>
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>vermelho</t>
+          <t>cinza</t>
         </is>
       </c>
       <c r="J95" t="n">
-        <v>95913</v>
+        <v>116891</v>
       </c>
     </row>
     <row r="96">
@@ -4633,16 +4633,16 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>diesel</t>
+          <t>flex</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -4651,7 +4651,7 @@
         </is>
       </c>
       <c r="G96" t="n">
-        <v>63703</v>
+        <v>26808</v>
       </c>
       <c r="H96" t="n">
         <v>2</v>
@@ -4662,18 +4662,18 @@
         </is>
       </c>
       <c r="J96" t="n">
-        <v>81140</v>
+        <v>77781</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Chevrolet</t>
+          <t>Toyota</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Tracker</t>
+          <t>Yaris</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -4686,42 +4686,42 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>etanol</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>automático</t>
+          <t>manual</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>87778</v>
+        <v>83727</v>
       </c>
       <c r="H97" t="n">
         <v>4</v>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J97" t="n">
-        <v>68851</v>
+        <v>57581</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>T-Cross</t>
+          <t>Tucson</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -4730,90 +4730,90 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>diesel</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>automático</t>
         </is>
       </c>
       <c r="G98" t="n">
-        <v>32285</v>
+        <v>47885</v>
       </c>
       <c r="H98" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>cinza</t>
+          <t>preto</t>
         </is>
       </c>
       <c r="J98" t="n">
-        <v>58543</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Volkswagen</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Polo</t>
+          <t>Tucson</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>2015</v>
+        <v>2019</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>gasolina</t>
+          <t>etanol</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>manual</t>
+          <t>CVT</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>37390</v>
+        <v>38665</v>
       </c>
       <c r="H99" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>prata</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J99" t="n">
-        <v>44929</v>
+        <v>99505</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Ford</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Hilux</t>
+          <t>EcoSport</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -4827,7 +4827,7 @@
         </is>
       </c>
       <c r="G100" t="n">
-        <v>81070</v>
+        <v>35145</v>
       </c>
       <c r="H100" t="n">
         <v>2</v>
@@ -4838,31 +4838,31 @@
         </is>
       </c>
       <c r="J100" t="n">
-        <v>115368</v>
+        <v>45155</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Toyota</t>
+          <t>Hyundai</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Yaris</t>
+          <t>Tucson</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>flex</t>
+          <t>gasolina</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -4871,18 +4871,18 @@
         </is>
       </c>
       <c r="G101" t="n">
-        <v>10206</v>
+        <v>62012</v>
       </c>
       <c r="H101" t="n">
         <v>2</v>
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>branco</t>
+          <t>vermelho</t>
         </is>
       </c>
       <c r="J101" t="n">
-        <v>89535</v>
+        <v>81477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>